<commit_message>
Update workflow configurations to trigger on 'not-main' branch and remove unused stage diagram workflow
</commit_message>
<xml_diff>
--- a/InputList/Acoustic/InputList.xlsx
+++ b/InputList/Acoustic/InputList.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Dev\TechnicalDocumentation\Input List\Acoustic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\InputList\Acoustic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{462CA518-7410-4610-9EC0-19807758E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44CE23A-21F4-4C78-B077-389417C76B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1305" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
   <sheets>
-    <sheet name="Input + Equipment" sheetId="1" r:id="rId1"/>
-    <sheet name="Snake + PA" sheetId="2" r:id="rId2"/>
+    <sheet name="Channels" sheetId="1" r:id="rId1"/>
+    <sheet name="Inputs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -740,6 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -803,6 +804,54 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -815,9 +864,6 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -827,52 +873,6 @@
     <xf numFmtId="0" fontId="11" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,7 +1351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -1369,33 +1369,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="e" vm="1">
+      <c r="A1" s="35" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="35"/>
+      <c r="C1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="28" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="29" t="str">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="30" t="str">
         <f ca="1">"Date Updated: "&amp;TEXT(TODAY(),"yyyy-mm-dd")</f>
-        <v>Date Updated: 2025-06-02</v>
-      </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
+        <v>Date Updated: 2026-02-10</v>
+      </c>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
@@ -1424,10 +1424,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>55</v>
       </c>
       <c r="C4" s="19">
@@ -1448,8 +1448,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
       <c r="C5" s="3">
         <v>2</v>
       </c>
@@ -1466,8 +1466,8 @@
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="41"/>
       <c r="C6" s="19">
         <v>3</v>
       </c>
@@ -1486,10 +1486,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="70" t="s">
+      <c r="A7" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="52" t="s">
         <v>56</v>
       </c>
       <c r="C7" s="20">
@@ -1510,8 +1510,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
-      <c r="B8" s="69"/>
+      <c r="A8" s="51"/>
+      <c r="B8" s="53"/>
       <c r="C8" s="21">
         <v>7</v>
       </c>
@@ -1528,22 +1528,22 @@
       <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="72"/>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72">
+      <c r="A9" s="28"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28">
         <v>8</v>
       </c>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
-      <c r="H9" s="72"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>57</v>
       </c>
       <c r="C10" s="6">
@@ -1564,8 +1564,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
       <c r="C11" s="7">
         <v>5</v>
       </c>
@@ -1582,10 +1582,10 @@
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="A12" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="46" t="s">
+      <c r="B12" s="47" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="24">
@@ -1606,8 +1606,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="47"/>
+      <c r="A13" s="45"/>
+      <c r="B13" s="48"/>
       <c r="C13" s="5">
         <v>10</v>
       </c>
@@ -1624,8 +1624,8 @@
       <c r="H13" s="5"/>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="48"/>
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="24">
         <v>11</v>
       </c>
@@ -1642,10 +1642,10 @@
       <c r="H14" s="24"/>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>59</v>
       </c>
       <c r="C15" s="26">
@@ -1666,8 +1666,8 @@
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="31"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="25">
         <v>12</v>
       </c>
@@ -1684,8 +1684,8 @@
       <c r="H16" s="25"/>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="26">
         <v>13</v>
       </c>
@@ -1702,8 +1702,8 @@
       <c r="H17" s="26"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="25">
         <v>14</v>
       </c>
@@ -1779,7 +1779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036672A4-8952-44C6-9E0D-0D4906E8D835}">
   <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
@@ -1799,78 +1799,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="e" vm="1">
+      <c r="A1" s="35" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="36" t="str">
-        <f>'Input + Equipment'!C1</f>
+      <c r="B1" s="35"/>
+      <c r="C1" s="37" t="str">
+        <f>Channels!C1</f>
         <v>Acoustic Setup</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="28" t="str">
-        <f>'Input + Equipment'!F1</f>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="29" t="str">
+        <f>Channels!F1</f>
         <v>www.theperfectstrangers.band</v>
       </c>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="28" t="str">
-        <f ca="1">'Input + Equipment'!F2</f>
-        <v>Date Updated: 2025-06-02</v>
-      </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
+      <c r="K2" s="29" t="str">
+        <f ca="1">Channels!F2</f>
+        <v>Date Updated: 2026-02-10</v>
+      </c>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="53" t="s">
+      <c r="A3" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="53"/>
-      <c r="C3" s="53"/>
-      <c r="D3" s="53"/>
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
       <c r="I3" s="11"/>
-      <c r="K3" s="52" t="s">
+      <c r="K3" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="52"/>
+      <c r="L3" s="69"/>
     </row>
     <row r="4" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="53"/>
-      <c r="E4" s="53"/>
-      <c r="F4" s="53"/>
-      <c r="G4" s="53"/>
-      <c r="H4" s="53"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="65"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="11"/>
       <c r="K4" s="16" t="s">
         <v>7</v>
@@ -1913,26 +1913,26 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="63" t="s">
+      <c r="C6" s="60"/>
+      <c r="D6" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="63" t="s">
+      <c r="E6" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="62" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="H6" s="60" t="s">
+      <c r="H6" s="62" t="s">
         <v>35</v>
       </c>
       <c r="I6" s="11"/>
@@ -1944,14 +1944,14 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
+      <c r="A7" s="71"/>
+      <c r="B7" s="72"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
       <c r="I7" s="11"/>
       <c r="K7" s="27">
         <v>3</v>
@@ -2001,28 +2001,28 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="A10" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="49" t="s">
+      <c r="B10" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="51" t="s">
+      <c r="E10" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="F10" s="51" t="s">
+      <c r="F10" s="68" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="62" t="s">
+      <c r="H10" s="57" t="s">
         <v>37</v>
       </c>
       <c r="I10" s="11"/>
@@ -2034,14 +2034,14 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="50"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="62"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="67"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="11"/>
       <c r="K11" s="24">
         <v>7</v>
@@ -2060,16 +2060,16 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="53"/>
-      <c r="D13" s="53"/>
-      <c r="E13" s="53"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="65"/>
       <c r="I13" s="11"/>
       <c r="K13" s="26">
         <v>9</v>
@@ -2115,17 +2115,17 @@
       <c r="A15" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="66" t="s">
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="G15" s="62" t="s">
+      <c r="G15" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="62" t="s">
+      <c r="H15" s="57" t="s">
         <v>40</v>
       </c>
       <c r="I15" s="11"/>
@@ -2139,13 +2139,13 @@
     </row>
     <row r="16" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="59"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
-      <c r="E16" s="58"/>
-      <c r="F16" s="66"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="56"/>
+      <c r="G16" s="57"/>
+      <c r="H16" s="57"/>
       <c r="I16" s="11"/>
       <c r="K16" s="26">
         <v>12</v>
@@ -2218,79 +2218,79 @@
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I23" s="11"/>
-      <c r="K23" s="67" t="s">
+      <c r="K23" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="L23" s="67"/>
-      <c r="M23" s="67"/>
-      <c r="N23" s="67"/>
-      <c r="O23" s="67"/>
+      <c r="L23" s="58"/>
+      <c r="M23" s="58"/>
+      <c r="N23" s="58"/>
+      <c r="O23" s="58"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I24" s="11"/>
       <c r="K24" s="4">
         <v>1</v>
       </c>
-      <c r="L24" s="65" t="s">
+      <c r="L24" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="M24" s="65"/>
-      <c r="N24" s="65"/>
-      <c r="O24" s="65"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="55"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I25" s="11"/>
       <c r="K25" s="2">
         <v>2</v>
       </c>
-      <c r="L25" s="64" t="s">
+      <c r="L25" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="M25" s="64"/>
-      <c r="N25" s="64"/>
-      <c r="O25" s="64"/>
+      <c r="M25" s="54"/>
+      <c r="N25" s="54"/>
+      <c r="O25" s="54"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
       <c r="K26" s="4">
         <v>3</v>
       </c>
-      <c r="L26" s="65" t="s">
+      <c r="L26" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="M26" s="65"/>
-      <c r="N26" s="65"/>
-      <c r="O26" s="65"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
+      <c r="O26" s="55"/>
     </row>
     <row r="27" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I27" s="11"/>
       <c r="K27" s="2">
         <v>4</v>
       </c>
-      <c r="L27" s="64"/>
-      <c r="M27" s="64"/>
-      <c r="N27" s="64"/>
-      <c r="O27" s="64"/>
+      <c r="L27" s="54"/>
+      <c r="M27" s="54"/>
+      <c r="N27" s="54"/>
+      <c r="O27" s="54"/>
     </row>
     <row r="28" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I28" s="11"/>
       <c r="K28" s="4">
         <v>5</v>
       </c>
-      <c r="L28" s="65"/>
-      <c r="M28" s="65"/>
-      <c r="N28" s="65"/>
-      <c r="O28" s="65"/>
+      <c r="L28" s="55"/>
+      <c r="M28" s="55"/>
+      <c r="N28" s="55"/>
+      <c r="O28" s="55"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I29" s="11"/>
       <c r="K29" s="2">
         <v>6</v>
       </c>
-      <c r="L29" s="64"/>
-      <c r="M29" s="64"/>
-      <c r="N29" s="64"/>
-      <c r="O29" s="64"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2300,16 +2300,19 @@
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="L27:O27"/>
-    <mergeCell ref="L28:O28"/>
-    <mergeCell ref="L29:O29"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="K23:O23"/>
-    <mergeCell ref="L24:O24"/>
-    <mergeCell ref="L25:O25"/>
-    <mergeCell ref="L26:O26"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="K3:L3"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="K1:O1"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="A15:A16"/>
@@ -2326,19 +2329,16 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="D6:D7"/>
     <mergeCell ref="A13:H13"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="K3:L3"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="L27:O27"/>
+    <mergeCell ref="L28:O28"/>
+    <mergeCell ref="L29:O29"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="K23:O23"/>
+    <mergeCell ref="L24:O24"/>
+    <mergeCell ref="L25:O25"/>
+    <mergeCell ref="L26:O26"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>